<commit_message>
Add Feedback and some function Service
</commit_message>
<xml_diff>
--- a/documnet/doanTN.xlsx
+++ b/documnet/doanTN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NhutDu\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\tailieu\DATN\SBike\documnet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="157">
   <si>
     <t>User</t>
   </si>
@@ -557,6 +557,9 @@
     <t>error : boolean
 data : feedback
 message : String</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -716,6 +719,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -733,12 +742,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1020,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E78"/>
+  <dimension ref="B3:F78"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1034,11 +1037,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
@@ -1235,16 +1238,16 @@
       <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="14" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="18"/>
     </row>
     <row r="28" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
@@ -1339,11 +1342,11 @@
       <c r="D37" s="8"/>
     </row>
     <row r="41" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="16"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="18"/>
       <c r="E41" t="s">
         <v>20</v>
       </c>
@@ -1378,11 +1381,11 @@
       <c r="D44" s="8"/>
     </row>
     <row r="47" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="16"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="18"/>
     </row>
     <row r="48" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="3" t="s">
@@ -1519,14 +1522,14 @@
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="65" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="14" t="s">
+    <row r="65" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C65" s="15"/>
-      <c r="D65" s="16"/>
-    </row>
-    <row r="66" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C65" s="17"/>
+      <c r="D65" s="18"/>
+    </row>
+    <row r="66" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="3" t="s">
         <v>1</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="2:4" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:6" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="8" t="s">
         <v>23</v>
       </c>
@@ -1546,7 +1549,7 @@
       </c>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="2:4" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:6" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="8" t="s">
         <v>25</v>
       </c>
@@ -1555,7 +1558,7 @@
       </c>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="2:4" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:6" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="8" t="s">
         <v>48</v>
       </c>
@@ -1565,8 +1568,11 @@
       <c r="D69" s="8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="70" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F69" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="s">
         <v>57</v>
       </c>
@@ -1575,7 +1581,7 @@
       </c>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="2:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="s">
         <v>58</v>
       </c>
@@ -1584,14 +1590,14 @@
       </c>
       <c r="D71" s="1"/>
     </row>
-    <row r="74" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="14" t="s">
+    <row r="74" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="16"/>
-    </row>
-    <row r="75" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C74" s="17"/>
+      <c r="D74" s="18"/>
+    </row>
+    <row r="75" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="4" t="s">
         <v>1</v>
       </c>
@@ -1602,7 +1608,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="76" spans="2:4" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:6" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="9" t="s">
         <v>23</v>
       </c>
@@ -1611,7 +1617,7 @@
       </c>
       <c r="D76" s="9"/>
     </row>
-    <row r="77" spans="2:4" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:6" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="9" t="s">
         <v>37</v>
       </c>
@@ -1620,7 +1626,7 @@
       </c>
       <c r="D77" s="9"/>
     </row>
-    <row r="78" spans="2:4" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:6" ht="20.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="9" t="s">
         <v>38</v>
       </c>
@@ -1647,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2057,10 +2063,10 @@
       <c r="D25" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="15" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2077,10 +2083,10 @@
       <c r="D26" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="15" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2097,10 +2103,10 @@
       <c r="D27" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="F27" s="21" t="s">
+      <c r="F27" s="15" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2129,19 +2135,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="G2" s="17" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="G2" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
     </row>
     <row r="3" spans="1:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">

</xml_diff>